<commit_message>
update new card images
</commit_message>
<xml_diff>
--- a/cardsJSONMaker.xlsx
+++ b/cardsJSONMaker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Documents\Rifftide\RifftideJSON\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Documents\Rifftide\RifftideSite\RifftideJSON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92725625-5A10-4370-84C4-97FFD74C8C6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B301587-2E51-4ACD-97EE-ED79B6D27735}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cards" sheetId="2" r:id="rId1"/>
@@ -21,9 +21,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="29">
   <si>
     <t>isaac</t>
   </si>
@@ -96,15 +94,9 @@
     <t>eventname</t>
   </si>
   <si>
-    <t>teal19</t>
-  </si>
-  <si>
     <t>dream</t>
   </si>
   <si>
-    <t>gold19</t>
-  </si>
-  <si>
     <t>hall19</t>
   </si>
   <si>
@@ -112,6 +104,18 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>Hymn of Christmas</t>
+  </si>
+  <si>
+    <t>christmas2019</t>
+  </si>
+  <si>
+    <t>teal2019</t>
+  </si>
+  <si>
+    <t>gold2019</t>
   </si>
 </sst>
 </file>
@@ -455,20 +459,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -488,16 +494,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.CONCAT(B2,"_",D2)</f>
-        <v>teal19_loryn</v>
+        <v>teal2019_loryn</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -511,16 +517,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C33" si="0">_xlfn.CONCAT(B3,"_",D3)</f>
-        <v>teal19_cara</v>
+        <f t="shared" ref="C3:C24" si="0">_xlfn.CONCAT(B3,"_",D3)</f>
+        <v>teal2019_cara</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
@@ -534,16 +540,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>teal19_bri</v>
+        <v>teal2019_bri</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -557,16 +563,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>teal19_laurel</v>
+        <v>teal2019_laurel</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -580,16 +586,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>teal19_zach</v>
+        <v>teal2019_zach</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
@@ -603,16 +609,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>teal19_isaac</v>
+        <v>teal2019_isaac</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -626,16 +632,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>teal19_johnnie</v>
+        <v>teal2019_johnnie</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -649,16 +655,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>teal19_sam</v>
+        <v>teal2019_sam</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -672,16 +678,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>gold19_loryn</v>
+        <v>gold2019_loryn</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -695,16 +701,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>gold19_cara</v>
+        <v>gold2019_cara</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
@@ -718,16 +724,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>gold19_bri</v>
+        <v>gold2019_bri</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -741,16 +747,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>gold19_laurel</v>
+        <v>gold2019_laurel</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -764,16 +770,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>gold19_zach</v>
+        <v>gold2019_zach</v>
       </c>
       <c r="D14" t="s">
         <v>1</v>
@@ -787,16 +793,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>gold19_isaac</v>
+        <v>gold2019_isaac</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
@@ -810,16 +816,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>gold19_johnnie</v>
+        <v>gold2019_johnnie</v>
       </c>
       <c r="D16" t="s">
         <v>3</v>
@@ -833,16 +839,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>gold19_sam</v>
+        <v>gold2019_sam</v>
       </c>
       <c r="D17" t="s">
         <v>4</v>
@@ -856,16 +862,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>hall19_loryn</v>
+        <v>christmas2019_loryn</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
@@ -879,349 +885,510 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>hall19_cara</v>
+        <v>christmas2019_bri</v>
       </c>
       <c r="D19" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E19">
         <f>VLOOKUP(D19,Sheet1!A:B,2,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19">
         <f>VLOOKUP(B19,Sheet1!E:F,2,FALSE)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C20" t="str">
-        <f>_xlfn.CONCAT(B20,"_",D20)</f>
-        <v>hall19_bri</v>
+        <f t="shared" si="0"/>
+        <v>christmas2019_laurel</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E20">
         <f>VLOOKUP(D20,Sheet1!A:B,2,FALSE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F20">
         <f>VLOOKUP(B20,Sheet1!E:F,2,FALSE)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>hall19_laurel</v>
+        <v>christmas2019_zach</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <f>VLOOKUP(D21,Sheet1!A:B,2,FALSE)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F21">
         <f>VLOOKUP(B21,Sheet1!E:F,2,FALSE)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>hall19_zach</v>
+        <v>christmas2019_isaac</v>
       </c>
       <c r="D22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <f>VLOOKUP(D22,Sheet1!A:B,2,FALSE)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F22">
         <f>VLOOKUP(B22,Sheet1!E:F,2,FALSE)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>hall19_isaac</v>
+        <v>christmas2019_johnnie</v>
       </c>
       <c r="D23" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E23">
         <f>VLOOKUP(D23,Sheet1!A:B,2,FALSE)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F23">
         <f>VLOOKUP(B23,Sheet1!E:F,2,FALSE)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>hall19_johnnie</v>
+        <v>christmas2019_sam</v>
       </c>
       <c r="D24" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24">
         <f>VLOOKUP(D24,Sheet1!A:B,2,FALSE)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F24">
         <f>VLOOKUP(B24,Sheet1!E:F,2,FALSE)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="0"/>
-        <v>hall19_sam</v>
+        <f>_xlfn.CONCAT(B25,"_",D25)</f>
+        <v>hall19_loryn</v>
       </c>
       <c r="D25" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E25">
         <f>VLOOKUP(D25,Sheet1!A:B,2,FALSE)</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F25">
         <f>VLOOKUP(B25,Sheet1!E:F,2,FALSE)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="0"/>
-        <v>dream_brennan</v>
+        <f>_xlfn.CONCAT(B26,"_",D26)</f>
+        <v>hall19_cara</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E26">
         <f>VLOOKUP(D26,Sheet1!A:B,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26">
         <f>VLOOKUP(B26,Sheet1!E:F,2,FALSE)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
         <v>22</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="0"/>
-        <v>dream_cara</v>
+        <f>_xlfn.CONCAT(B27,"_",D27)</f>
+        <v>hall19_bri</v>
       </c>
       <c r="D27" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E27">
         <f>VLOOKUP(D27,Sheet1!A:B,2,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27">
         <f>VLOOKUP(B27,Sheet1!E:F,2,FALSE)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
         <v>22</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="0"/>
-        <v>dream_bri</v>
+        <f>_xlfn.CONCAT(B28,"_",D28)</f>
+        <v>hall19_laurel</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E28">
         <f>VLOOKUP(D28,Sheet1!A:B,2,FALSE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F28">
         <f>VLOOKUP(B28,Sheet1!E:F,2,FALSE)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
         <v>22</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="0"/>
-        <v>dream_emily</v>
+        <f>_xlfn.CONCAT(B29,"_",D29)</f>
+        <v>hall19_zach</v>
       </c>
       <c r="D29" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E29">
         <f>VLOOKUP(D29,Sheet1!A:B,2,FALSE)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F29">
         <f>VLOOKUP(B29,Sheet1!E:F,2,FALSE)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
         <v>22</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="0"/>
-        <v>dream_zach</v>
+        <f>_xlfn.CONCAT(B30,"_",D30)</f>
+        <v>hall19_isaac</v>
       </c>
       <c r="D30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <f>VLOOKUP(D30,Sheet1!A:B,2,FALSE)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F30">
         <f>VLOOKUP(B30,Sheet1!E:F,2,FALSE)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
         <v>22</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="0"/>
-        <v>dream_isaac</v>
+        <f>_xlfn.CONCAT(B31,"_",D31)</f>
+        <v>hall19_johnnie</v>
       </c>
       <c r="D31" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E31">
         <f>VLOOKUP(D31,Sheet1!A:B,2,FALSE)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F31">
         <f>VLOOKUP(B31,Sheet1!E:F,2,FALSE)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
         <v>22</v>
       </c>
       <c r="C32" t="str">
-        <f t="shared" si="0"/>
-        <v>dream_johnnie</v>
+        <f>_xlfn.CONCAT(B32,"_",D32)</f>
+        <v>hall19_sam</v>
       </c>
       <c r="D32" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E32">
         <f>VLOOKUP(D32,Sheet1!A:B,2,FALSE)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F32">
         <f>VLOOKUP(B32,Sheet1!E:F,2,FALSE)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C33" t="str">
-        <f t="shared" si="0"/>
-        <v>dream_sam</v>
+        <f>_xlfn.CONCAT(B33,"_",D33)</f>
+        <v>dream_brennan</v>
       </c>
       <c r="D33" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E33">
         <f>VLOOKUP(D33,Sheet1!A:B,2,FALSE)</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F33">
         <f>VLOOKUP(B33,Sheet1!E:F,2,FALSE)</f>
-        <v>4</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="str">
+        <f>_xlfn.CONCAT(B34,"_",D34)</f>
+        <v>dream_cara</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <f>VLOOKUP(D34,Sheet1!A:B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <f>VLOOKUP(B34,Sheet1!E:F,2,FALSE)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" t="str">
+        <f>_xlfn.CONCAT(B35,"_",D35)</f>
+        <v>dream_bri</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <f>VLOOKUP(D35,Sheet1!A:B,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <f>VLOOKUP(B35,Sheet1!E:F,2,FALSE)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" t="str">
+        <f>_xlfn.CONCAT(B36,"_",D36)</f>
+        <v>dream_emily</v>
+      </c>
+      <c r="D36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36">
+        <f>VLOOKUP(D36,Sheet1!A:B,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <f>VLOOKUP(B36,Sheet1!E:F,2,FALSE)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" t="str">
+        <f>_xlfn.CONCAT(B37,"_",D37)</f>
+        <v>dream_zach</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <f>VLOOKUP(D37,Sheet1!A:B,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <f>VLOOKUP(B37,Sheet1!E:F,2,FALSE)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" t="str">
+        <f>_xlfn.CONCAT(B38,"_",D38)</f>
+        <v>dream_isaac</v>
+      </c>
+      <c r="D38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <f>VLOOKUP(D38,Sheet1!A:B,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="F38">
+        <f>VLOOKUP(B38,Sheet1!E:F,2,FALSE)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" t="str">
+        <f>_xlfn.CONCAT(B39,"_",D39)</f>
+        <v>dream_johnnie</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <f>VLOOKUP(D39,Sheet1!A:B,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="F39">
+        <f>VLOOKUP(B39,Sheet1!E:F,2,FALSE)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" t="str">
+        <f>_xlfn.CONCAT(B40,"_",D40)</f>
+        <v>dream_sam</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <f>VLOOKUP(D40,Sheet1!A:B,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="F40">
+        <f>VLOOKUP(B40,Sheet1!E:F,2,FALSE)</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1235,20 +1402,20 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
         <v>19</v>
@@ -1257,7 +1424,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1265,13 +1432,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1279,13 +1446,13 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1293,13 +1460,13 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1313,15 +1480,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1329,7 +1502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1337,7 +1510,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1345,7 +1518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1353,7 +1526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>

</xml_diff>